<commit_message>
Add setup for Isomer case and change the sintering file for is to be the same as that of BP
</commit_message>
<xml_diff>
--- a/INIT_files/InformationOfAutoinit.xlsx
+++ b/INIT_files/InformationOfAutoinit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zixianghong/Desktop/College Stuff/Heterogeneous Catalysis/Sintering-Project/INIT_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682D499B-A3BA-F342-889E-01F8FFF04591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD79D97-C57D-C741-8D9B-AD3C6646A5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21000" yWindow="7920" windowWidth="28240" windowHeight="17440" xr2:uid="{54CCC7FE-F371-5D49-B75A-0E96665D722F}"/>
+    <workbookView xWindow="6320" yWindow="760" windowWidth="28240" windowHeight="17440" xr2:uid="{54CCC7FE-F371-5D49-B75A-0E96665D722F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="218" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>